<commit_message>
pun Analyzed data and made graphs
</commit_message>
<xml_diff>
--- a/data/Metadata.xlsx
+++ b/data/Metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcbar\Documents\4th Year\Oban Field Course\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\EESField-Group5\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5BAE5C-0B6D-439B-BB4F-66CC6614B1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF71E9C-3581-44A1-8788-EB78F7A89D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{31F22BF3-83DF-4EB3-B33D-72A9C36649DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{31F22BF3-83DF-4EB3-B33D-72A9C36649DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
   <si>
     <t>Site number</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>NM 848 265</t>
+  </si>
+  <si>
+    <t>Alpha Diversity</t>
   </si>
 </sst>
 </file>
@@ -451,15 +454,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5FD38F-5954-46E9-803D-64ED511A1DB7}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,8 +487,11 @@
       <c r="H1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -507,8 +513,11 @@
       <c r="G2">
         <v>2907</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -530,8 +539,11 @@
       <c r="G3">
         <v>2911</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -553,8 +565,11 @@
       <c r="G4">
         <v>2913</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -576,8 +591,11 @@
       <c r="G5">
         <v>2914</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -599,8 +617,11 @@
       <c r="G6">
         <v>2915</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -622,8 +643,11 @@
       <c r="G7">
         <v>2918</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -645,8 +669,11 @@
       <c r="G8">
         <v>2919</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -668,8 +695,11 @@
       <c r="G9">
         <v>2920</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -691,8 +721,11 @@
       <c r="G10">
         <v>2921</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -714,8 +747,11 @@
       <c r="G11">
         <v>2923</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -737,8 +773,11 @@
       <c r="G12">
         <v>2926</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -760,8 +799,11 @@
       <c r="G13">
         <v>2928</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -783,8 +825,11 @@
       <c r="G14">
         <v>2930</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -806,8 +851,11 @@
       <c r="G15">
         <v>2931</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -829,8 +877,11 @@
       <c r="G16">
         <v>2932</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -852,8 +903,11 @@
       <c r="G17">
         <v>2933</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -875,8 +929,11 @@
       <c r="G18">
         <v>2934</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -898,8 +955,11 @@
       <c r="G19">
         <v>2935</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -921,8 +981,11 @@
       <c r="G20">
         <v>2936</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -944,8 +1007,11 @@
       <c r="G21">
         <v>2937</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -967,8 +1033,11 @@
       <c r="G22">
         <v>2941</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -990,8 +1059,11 @@
       <c r="G23">
         <v>2942</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1013,8 +1085,11 @@
       <c r="G24">
         <v>2943</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1036,8 +1111,11 @@
       <c r="G25">
         <v>2945</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1058,6 +1136,9 @@
       </c>
       <c r="G26">
         <v>2946</v>
+      </c>
+      <c r="I26">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1066,6 +1147,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010028531907D5E3F14D8CAA118412C77D47" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e1638c8c395ba01e38b44b2bd016668c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bbd738eb-4373-4af4-9565-43884bb1760c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="285c3851ef625c428f1ba8b8af604715" ns2:_="">
     <xsd:import namespace="bbd738eb-4373-4af4-9565-43884bb1760c"/>
@@ -1229,15 +1319,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1245,13 +1326,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CEEA096-C050-41DF-841B-1648C262B6B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D21BFFD3-2EBF-4D10-AC68-9195B5DCD196}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D21BFFD3-2EBF-4D10-AC68-9195B5DCD196}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CEEA096-C050-41DF-841B-1648C262B6B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bbd738eb-4373-4af4-9565-43884bb1760c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{969B8D27-52E2-45C0-AF2C-EF22BE627449}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{969B8D27-52E2-45C0-AF2C-EF22BE627449}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Metadata from James and Laura
</commit_message>
<xml_diff>
--- a/data/Metadata.xlsx
+++ b/data/Metadata.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\EESField-Group5\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\iona.sms.ed.ac.uk\home\s1837184\Github\EESField-Group5\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF71E9C-3581-44A1-8788-EB78F7A89D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{31F22BF3-83DF-4EB3-B33D-72A9C36649DD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,85 +33,106 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
-  <si>
-    <t>Site number</t>
-  </si>
-  <si>
-    <t>Grid ref.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="28">
+  <si>
+    <t>Plot_number</t>
+  </si>
+  <si>
+    <t>Grid_ref.</t>
   </si>
   <si>
     <t>LUX</t>
   </si>
   <si>
-    <t>Overstorey Species</t>
+    <t>Overstorey_Species</t>
   </si>
   <si>
     <t>Weather</t>
   </si>
   <si>
-    <t>File name</t>
+    <t>Stems_in_10m_radius_circular plot</t>
+  </si>
+  <si>
+    <t>File_name</t>
+  </si>
+  <si>
+    <t>Mean_reading%</t>
+  </si>
+  <si>
+    <t>pH_readings</t>
   </si>
   <si>
     <t>NM 851 263</t>
   </si>
   <si>
+    <t>Sitka spruce</t>
+  </si>
+  <si>
+    <t>Raining, overcast</t>
+  </si>
+  <si>
+    <t>Soil_moisture_1</t>
+  </si>
+  <si>
+    <t>Soil_moisture_2</t>
+  </si>
+  <si>
+    <t>Soil_moisture_3</t>
+  </si>
+  <si>
+    <t>Soil_moisture_4</t>
+  </si>
+  <si>
     <t>NM 851 262</t>
   </si>
   <si>
+    <t>Scots pine with Sitka either side</t>
+  </si>
+  <si>
     <t>NM 850 264</t>
   </si>
   <si>
+    <t>Larch</t>
+  </si>
+  <si>
+    <t>Lightly raining</t>
+  </si>
+  <si>
     <t>NM 850 263</t>
   </si>
   <si>
+    <t>Sitka spruce and scots pine</t>
+  </si>
+  <si>
+    <t>&gt;85</t>
+  </si>
+  <si>
+    <t>Overcast but dry</t>
+  </si>
+  <si>
     <t>NM 849 264</t>
   </si>
   <si>
-    <t>Sitka spruce</t>
-  </si>
-  <si>
-    <t>Scots pine with Sitka either side</t>
-  </si>
-  <si>
-    <t>Larch</t>
-  </si>
-  <si>
-    <t>Raining, overcast</t>
-  </si>
-  <si>
-    <t>Lightly raining</t>
-  </si>
-  <si>
-    <t>Sitka spruce and scots pine</t>
-  </si>
-  <si>
-    <t>Overcast but dry</t>
-  </si>
-  <si>
     <t>Scotspine with Larch and scots pine either side. Rowan trees also directly East.</t>
   </si>
   <si>
-    <t>Number of trees in plot</t>
-  </si>
-  <si>
-    <t>Stocking density</t>
-  </si>
-  <si>
     <t>NM 848 265</t>
-  </si>
-  <si>
-    <t>Alpha Diversity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -453,16 +473,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5FD38F-5954-46E9-803D-64ED511A1DB7}">
-  <dimension ref="A1:I26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,33 +504,48 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>94.7</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -513,25 +553,44 @@
       <c r="G2">
         <v>2907</v>
       </c>
+      <c r="H2">
+        <f>P3</f>
+        <v>0</v>
+      </c>
       <c r="I2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>25.4</v>
+      </c>
+      <c r="L2">
+        <v>26.9</v>
+      </c>
+      <c r="M2">
+        <v>19</v>
+      </c>
+      <c r="N2">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>111.8</v>
       </c>
       <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
       <c r="F3">
         <v>43</v>
@@ -539,25 +598,44 @@
       <c r="G3">
         <v>2911</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H26" si="0">P4</f>
+        <v>0</v>
+      </c>
       <c r="I3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>24.2</v>
+      </c>
+      <c r="L3">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="M3">
+        <v>38.6</v>
+      </c>
+      <c r="N3">
+        <v>43.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>99.6</v>
       </c>
       <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
       </c>
       <c r="F4">
         <v>54</v>
@@ -565,25 +643,44 @@
       <c r="G4">
         <v>2913</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>14.6</v>
+      </c>
+      <c r="L4">
+        <v>10.9</v>
+      </c>
+      <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>318</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F5">
         <v>30</v>
@@ -591,25 +688,44 @@
       <c r="G5">
         <v>2914</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>15.6</v>
+      </c>
+      <c r="L5">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="M5">
+        <v>58.7</v>
+      </c>
+      <c r="N5">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>65.900000000000006</v>
       </c>
       <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
       </c>
       <c r="F6">
         <v>63</v>
@@ -617,25 +733,44 @@
       <c r="G6">
         <v>2915</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I6">
+        <v>4.5</v>
+      </c>
+      <c r="J6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>22.4</v>
+      </c>
+      <c r="L6">
+        <v>52</v>
+      </c>
+      <c r="M6">
+        <v>26.6</v>
+      </c>
+      <c r="N6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>169.3</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <v>27</v>
@@ -643,25 +778,44 @@
       <c r="G7">
         <v>2918</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.5</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>11.3</v>
+      </c>
+      <c r="L7">
+        <v>42.3</v>
+      </c>
+      <c r="M7">
+        <v>84.3</v>
+      </c>
+      <c r="N7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>270</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F8">
         <v>30</v>
@@ -669,25 +823,44 @@
       <c r="G8">
         <v>2919</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.5</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>20.6</v>
+      </c>
+      <c r="L8">
+        <v>21.5</v>
+      </c>
+      <c r="M8">
+        <v>14.2</v>
+      </c>
+      <c r="N8">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>1430</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F9">
         <v>21</v>
@@ -695,25 +868,44 @@
       <c r="G9">
         <v>2920</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>66.8</v>
+      </c>
+      <c r="L9">
+        <v>53.7</v>
+      </c>
+      <c r="M9">
+        <v>64.2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>1618</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F10">
         <v>33</v>
@@ -721,25 +913,44 @@
       <c r="G10">
         <v>2921</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.5</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>1756</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>14</v>
@@ -747,25 +958,44 @@
       <c r="G11">
         <v>2923</v>
       </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11">
+        <v>52.2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>20200</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F12">
         <v>42</v>
@@ -773,25 +1003,44 @@
       <c r="G12">
         <v>2926</v>
       </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <v>60</v>
+      </c>
+      <c r="L12">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="M12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>88.1</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F13">
         <v>52</v>
@@ -799,25 +1048,44 @@
       <c r="G13">
         <v>2928</v>
       </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>19.2</v>
+      </c>
+      <c r="L13">
+        <v>6.4</v>
+      </c>
+      <c r="M13">
+        <v>30.8</v>
+      </c>
+      <c r="N13">
+        <v>47.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>276</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F14">
         <v>48</v>
@@ -825,25 +1093,44 @@
       <c r="G14">
         <v>2930</v>
       </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I14">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J14">
+        <v>13</v>
+      </c>
+      <c r="K14">
+        <v>24.9</v>
+      </c>
+      <c r="L14">
+        <v>52.4</v>
+      </c>
+      <c r="M14">
+        <v>65.5</v>
+      </c>
+      <c r="N14">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>1950</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F15">
         <v>42</v>
@@ -851,25 +1138,44 @@
       <c r="G15">
         <v>2931</v>
       </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K15">
+        <v>51.7</v>
+      </c>
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C16">
         <v>187</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F16">
         <v>33</v>
@@ -877,25 +1183,44 @@
       <c r="G16">
         <v>2932</v>
       </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J16">
+        <v>15</v>
+      </c>
+      <c r="K16">
+        <v>18.5</v>
+      </c>
+      <c r="L16">
+        <v>52.6</v>
+      </c>
+      <c r="M16">
+        <v>27</v>
+      </c>
+      <c r="N16">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C17">
         <v>282</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F17">
         <v>35</v>
@@ -903,25 +1228,44 @@
       <c r="G17">
         <v>2933</v>
       </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J17">
+        <v>16</v>
+      </c>
+      <c r="K17">
+        <v>23.9</v>
+      </c>
+      <c r="L17">
+        <v>20</v>
+      </c>
+      <c r="M17">
+        <v>35.9</v>
+      </c>
+      <c r="N17">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>39.799999999999997</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>63</v>
@@ -929,25 +1273,44 @@
       <c r="G18">
         <v>2934</v>
       </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J18">
+        <v>17</v>
+      </c>
+      <c r="K18">
+        <v>18.7</v>
+      </c>
+      <c r="L18">
+        <v>20.7</v>
+      </c>
+      <c r="M18">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="N18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F19">
         <v>49</v>
@@ -955,25 +1318,44 @@
       <c r="G19">
         <v>2935</v>
       </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J19">
+        <v>18</v>
+      </c>
+      <c r="K19">
+        <v>41.2</v>
+      </c>
+      <c r="L19">
+        <v>24.7</v>
+      </c>
+      <c r="M19">
+        <v>34</v>
+      </c>
+      <c r="N19">
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F20">
         <v>49</v>
@@ -981,25 +1363,44 @@
       <c r="G20">
         <v>2936</v>
       </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.5</v>
+      </c>
+      <c r="J20">
+        <v>19</v>
+      </c>
+      <c r="K20">
+        <v>23.6</v>
+      </c>
+      <c r="L20">
+        <v>29.6</v>
+      </c>
+      <c r="M20">
+        <v>22.6</v>
+      </c>
+      <c r="N20">
+        <v>33.200000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <v>338</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F21">
         <v>46</v>
@@ -1007,25 +1408,44 @@
       <c r="G21">
         <v>2937</v>
       </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J21">
+        <v>20</v>
+      </c>
+      <c r="K21">
+        <v>30.2</v>
+      </c>
+      <c r="L21">
+        <v>21.4</v>
+      </c>
+      <c r="M21">
+        <v>23.8</v>
+      </c>
+      <c r="N21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>292</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F22">
         <v>45</v>
@@ -1033,25 +1453,44 @@
       <c r="G22">
         <v>2941</v>
       </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="J22">
+        <v>21</v>
+      </c>
+      <c r="K22">
+        <v>28.2</v>
+      </c>
+      <c r="L22">
+        <v>27.3</v>
+      </c>
+      <c r="M22">
+        <v>56</v>
+      </c>
+      <c r="N22">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>164</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F23">
         <v>52</v>
@@ -1059,25 +1498,44 @@
       <c r="G23">
         <v>2942</v>
       </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J23">
+        <v>22</v>
+      </c>
+      <c r="K23">
+        <v>40.4</v>
+      </c>
+      <c r="L23">
+        <v>70.3</v>
+      </c>
+      <c r="M23">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="N23">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>147</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F24">
         <v>62</v>
@@ -1085,25 +1543,44 @@
       <c r="G24">
         <v>2943</v>
       </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J24">
+        <v>23</v>
+      </c>
+      <c r="K24">
+        <v>19</v>
+      </c>
+      <c r="L24">
+        <v>9.1</v>
+      </c>
+      <c r="M24">
+        <v>14.8</v>
+      </c>
+      <c r="N24">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>260</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F25">
         <v>59</v>
@@ -1111,25 +1588,44 @@
       <c r="G25">
         <v>2945</v>
       </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I25">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+      <c r="J25">
+        <v>24</v>
+      </c>
+      <c r="K25">
+        <v>22.8</v>
+      </c>
+      <c r="L25">
+        <v>18.2</v>
+      </c>
+      <c r="M25">
+        <v>29.6</v>
+      </c>
+      <c r="N25">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>149</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F26">
         <v>60</v>
@@ -1137,11 +1633,31 @@
       <c r="G26">
         <v>2946</v>
       </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I26">
-        <v>9</v>
+        <v>4.5</v>
+      </c>
+      <c r="J26">
+        <v>25</v>
+      </c>
+      <c r="K26">
+        <v>47.6</v>
+      </c>
+      <c r="L26">
+        <v>26.8</v>
+      </c>
+      <c r="M26">
+        <v>27.3</v>
+      </c>
+      <c r="N26">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1156,8 +1672,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010028531907D5E3F14D8CAA118412C77D47" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e1638c8c395ba01e38b44b2bd016668c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bbd738eb-4373-4af4-9565-43884bb1760c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="285c3851ef625c428f1ba8b8af604715" ns2:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010028531907D5E3F14D8CAA118412C77D47" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="69dd7a871a24e623b61af56c3cd7242a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bbd738eb-4373-4af4-9565-43884bb1760c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56ded60a1efe100aa9dcd0eabdd1bc1" ns2:_="">
     <xsd:import namespace="bbd738eb-4373-4af4-9565-43884bb1760c"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -1172,6 +1694,7 @@
                 <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1217,6 +1740,13 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1319,14 +1849,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D21BFFD3-2EBF-4D10-AC68-9195B5DCD196}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D87BBBAF-A519-496F-A4B7-0C42207D0EA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
@@ -1334,7 +1858,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CEEA096-C050-41DF-841B-1648C262B6B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E113C6C-6425-4628-96FF-0FBAE312EF24}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9057825A-76C5-4E43-AB96-B64D94B0EAB5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -1349,13 +1882,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{969B8D27-52E2-45C0-AF2C-EF22BE627449}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>